<commit_message>
Remove highlighting from PhosFate output
</commit_message>
<xml_diff>
--- a/Results/enrichment/phosfate_output.xlsx
+++ b/Results/enrichment/phosfate_output.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agitter\Desktop\madison\collaborators\Ahlquist\hiv\hiv1-aurkb\Results\enrichment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF77F248-3F84-486B-96A8-F6F8B70DB943}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="kinase activities 5 min" sheetId="1" r:id="rId1"/>
@@ -489,7 +488,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,6 +619,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -966,9 +971,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1326,13 +1332,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1349,7 +1353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>35</v>
       </c>
@@ -1366,7 +1370,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1383,7 +1387,7 @@
         <v>-2.2218487496163499</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>14</v>
       </c>
@@ -1400,92 +1404,92 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>-0.83989279349762103</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>-1.82390874094431</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>-0.82785493056249304</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>-1.7695510786217199</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="1">
         <v>28</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>-0.450516996883009</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0.02</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>-1.6989700043360101</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="2">
         <v>23</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>-0.50061262642469395</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>2.3E-2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>-1.6382721639824001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
         <v>-0.97143427886536104</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>-1.49485002168009</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1502,7 +1506,7 @@
         <v>-1.48148606012211</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1519,7 +1523,7 @@
         <v>-1.4089353929735</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1536,7 +1540,7 @@
         <v>-1.27572413039921</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1553,7 +1557,7 @@
         <v>-1.2596373105057499</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1570,7 +1574,7 @@
         <v>-1.1366771398795401</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1587,7 +1591,7 @@
         <v>-1.13076828026902</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1604,7 +1608,7 @@
         <v>-1.1079053973095101</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1621,7 +1625,7 @@
         <v>-1.0506099933550801</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1638,7 +1642,7 @@
         <v>-1.0409586076788999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1655,7 +1659,7 @@
         <v>-0.98296666070121896</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1672,7 +1676,7 @@
         <v>-0.97061622231478994</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1689,7 +1693,7 @@
         <v>-0.95860731484177497</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1706,7 +1710,7 @@
         <v>-0.95078197732981795</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1723,7 +1727,7 @@
         <v>-0.93554201077308097</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1740,7 +1744,7 @@
         <v>-0.882728704344235</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1757,7 +1761,7 @@
         <v>-0.87942606879414997</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1774,7 +1778,7 @@
         <v>-0.82102305270682996</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1791,7 +1795,7 @@
         <v>-0.81247927916353602</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1808,7 +1812,7 @@
         <v>-0.80966830182970795</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1825,7 +1829,7 @@
         <v>-0.79860287567954802</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1842,7 +1846,7 @@
         <v>-0.77469071827413705</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1859,7 +1863,7 @@
         <v>-0.772113295386326</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>17</v>
       </c>
@@ -1876,7 +1880,7 @@
         <v>-0.75696195131370503</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1893,7 +1897,7 @@
         <v>-0.73992861201492499</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1910,7 +1914,7 @@
         <v>-0.72815839346350097</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1927,7 +1931,7 @@
         <v>-0.71219827006977399</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>10</v>
       </c>
@@ -1944,7 +1948,7 @@
         <v>-0.70996538863748104</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1961,7 +1965,7 @@
         <v>-0.69250396208678699</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1978,7 +1982,7 @@
         <v>-0.69250396208678699</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>-0.68824613894424502</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2012,7 +2016,7 @@
         <v>-0.68402965454308196</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2029,7 +2033,7 @@
         <v>-0.67162039656126205</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2046,7 +2050,7 @@
         <v>-0.66958622665080902</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>2</v>
       </c>
@@ -2063,7 +2067,7 @@
         <v>-0.651695136951839</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2080,7 +2084,7 @@
         <v>-0.62708799702989304</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>5</v>
       </c>
@@ -2097,7 +2101,7 @@
         <v>-0.62342304294348805</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>1</v>
       </c>
@@ -2114,7 +2118,7 @@
         <v>-0.62342304294348805</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>28</v>
       </c>
@@ -2131,7 +2135,7 @@
         <v>-0.59859945921845503</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>1</v>
       </c>
@@ -2148,7 +2152,7 @@
         <v>-0.59859945921845503</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>45</v>
       </c>
@@ -2165,7 +2169,7 @@
         <v>-0.58335949266171905</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>5</v>
       </c>
@@ -2182,7 +2186,7 @@
         <v>-0.57839607313016805</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>2</v>
       </c>
@@ -2199,7 +2203,7 @@
         <v>-0.515700160653214</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>1</v>
       </c>
@@ -2216,7 +2220,7 @@
         <v>-0.50863830616572703</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>2</v>
       </c>
@@ -2233,7 +2237,7 @@
         <v>-0.48545224733971298</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>10</v>
       </c>
@@ -2250,7 +2254,7 @@
         <v>-0.47237009912866101</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>1</v>
       </c>
@@ -2267,7 +2271,7 @@
         <v>-0.45967052520912599</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>1</v>
       </c>
@@ -2284,7 +2288,7 @@
         <v>-0.44977164694490501</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2301,7 +2305,7 @@
         <v>-0.44611697335612499</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>1</v>
       </c>
@@ -2318,7 +2322,7 @@
         <v>-0.42481215507233799</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>6</v>
       </c>
@@ -2335,7 +2339,7 @@
         <v>-0.41907502432437999</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2352,7 +2356,7 @@
         <v>-0.406713932979542</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>12</v>
       </c>
@@ -2369,7 +2373,7 @@
         <v>-0.40011692792631198</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>1</v>
       </c>
@@ -2386,7 +2390,7 @@
         <v>-0.38090666937325701</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>2</v>
       </c>
@@ -2403,7 +2407,7 @@
         <v>-0.37778597703370398</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>2</v>
       </c>
@@ -2420,7 +2424,7 @@
         <v>-0.34582345812203902</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>1</v>
       </c>
@@ -2437,7 +2441,7 @@
         <v>-0.341988603342887</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>4</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>-0.33913452199612998</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>1</v>
       </c>
@@ -2471,7 +2475,7 @@
         <v>-0.30891850787703101</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>9</v>
       </c>
@@ -2488,7 +2492,7 @@
         <v>0.27245874297144301</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>14</v>
       </c>
@@ -2505,7 +2509,7 @@
         <v>0.318758762624412</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>5</v>
       </c>
@@ -2522,7 +2526,7 @@
         <v>0.320572103387881</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>2</v>
       </c>
@@ -2539,7 +2543,7 @@
         <v>0.32975414692587501</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>1</v>
       </c>
@@ -2556,7 +2560,7 @@
         <v>0.33535802444387403</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>3</v>
       </c>
@@ -2573,7 +2577,7 @@
         <v>0.36151074304536202</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>1</v>
       </c>
@@ -2590,7 +2594,7 @@
         <v>0.36653154442041302</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>1</v>
       </c>
@@ -2607,7 +2611,7 @@
         <v>0.39361863488939502</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>1</v>
       </c>
@@ -2624,7 +2628,7 @@
         <v>0.39577394691552897</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>7</v>
       </c>
@@ -2641,7 +2645,7 @@
         <v>0.40120949323688399</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>4</v>
       </c>
@@ -2658,7 +2662,7 @@
         <v>0.40230481407448698</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>1</v>
       </c>
@@ -2675,7 +2679,7 @@
         <v>0.40230481407448698</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>3</v>
       </c>
@@ -2692,7 +2696,7 @@
         <v>0.41005039867429199</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>1</v>
       </c>
@@ -2709,7 +2713,7 @@
         <v>0.41680122603137698</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>1</v>
       </c>
@@ -2726,7 +2730,7 @@
         <v>0.421360790031927</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>1</v>
       </c>
@@ -2743,7 +2747,7 @@
         <v>0.42596873227228099</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>1</v>
       </c>
@@ -2760,7 +2764,7 @@
         <v>0.43770713554352503</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>1</v>
       </c>
@@ -2777,7 +2781,7 @@
         <v>0.43889861635094402</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>1</v>
       </c>
@@ -2794,7 +2798,7 @@
         <v>0.44009337496388701</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>1</v>
       </c>
@@ -2811,7 +2815,7 @@
         <v>0.455931955649724</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>12</v>
       </c>
@@ -2828,7 +2832,7 @@
         <v>0.46092390120722299</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>6</v>
       </c>
@@ -2845,7 +2849,7 @@
         <v>0.52287874528033695</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>1</v>
       </c>
@@ -2862,7 +2866,7 @@
         <v>0.52870828894106103</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>4</v>
       </c>
@@ -2879,7 +2883,7 @@
         <v>0.54211810326600696</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>1</v>
       </c>
@@ -2896,7 +2900,7 @@
         <v>0.58502665202918203</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>3</v>
       </c>
@@ -2913,7 +2917,7 @@
         <v>0.59345981956604399</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>1</v>
       </c>
@@ -2930,7 +2934,7 @@
         <v>0.61798295742513099</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>1</v>
       </c>
@@ -2947,7 +2951,7 @@
         <v>0.63451201510910005</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>1</v>
       </c>
@@ -2964,7 +2968,7 @@
         <v>0.64016451766011195</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>1</v>
       </c>
@@ -2981,7 +2985,7 @@
         <v>0.64397414280687704</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>2</v>
       </c>
@@ -2998,7 +3002,7 @@
         <v>0.66958622665080902</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>8</v>
       </c>
@@ -3015,7 +3019,7 @@
         <v>0.66958622665080902</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>1</v>
       </c>
@@ -3032,7 +3036,7 @@
         <v>0.68402965454308196</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>5</v>
       </c>
@@ -3049,7 +3053,7 @@
         <v>0.68613277963084596</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>2</v>
       </c>
@@ -3066,7 +3070,7 @@
         <v>0.68613277963084596</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>2</v>
       </c>
@@ -3083,7 +3087,7 @@
         <v>0.71669877129644999</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>1</v>
       </c>
@@ -3100,7 +3104,7 @@
         <v>0.72124639904717103</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>17</v>
       </c>
@@ -3117,7 +3121,7 @@
         <v>0.72584215073631997</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>1</v>
       </c>
@@ -3134,7 +3138,7 @@
         <v>0.72815839346350097</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>2</v>
       </c>
@@ -3151,7 +3155,7 @@
         <v>0.73518217699046295</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>1</v>
       </c>
@@ -3168,7 +3172,7 @@
         <v>0.75945075171739995</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>2</v>
       </c>
@@ -3185,7 +3189,7 @@
         <v>0.76447155309245096</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A110">
         <v>7</v>
       </c>
@@ -3202,7 +3206,7 @@
         <v>0.78515615195230204</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>2</v>
       </c>
@@ -3219,7 +3223,7 @@
         <v>0.80410034759076598</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>17</v>
       </c>
@@ -3236,7 +3240,7 @@
         <v>0.80687540164553795</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A113">
         <v>2</v>
       </c>
@@ -3253,7 +3257,7 @@
         <v>0.82681373158772598</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A114">
         <v>3</v>
       </c>
@@ -3270,7 +3274,7 @@
         <v>0.85387196432176105</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A115">
         <v>2</v>
       </c>
@@ -3287,7 +3291,7 @@
         <v>0.85698519974590404</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A116">
         <v>1</v>
       </c>
@@ -3304,7 +3308,7 @@
         <v>0.87614835903291399</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A117">
         <v>2</v>
       </c>
@@ -3321,7 +3325,7 @@
         <v>0.90657831483776496</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A118">
         <v>7</v>
       </c>
@@ -3338,7 +3342,7 @@
         <v>0.93554201077308097</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>1</v>
       </c>
@@ -3355,7 +3359,7 @@
         <v>0.97881070093006195</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A120">
         <v>3</v>
       </c>
@@ -3372,7 +3376,7 @@
         <v>1.0132282657337499</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A121">
         <v>3</v>
       </c>
@@ -3389,7 +3393,7 @@
         <v>1.0409586076788999</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A122">
         <v>26</v>
       </c>
@@ -3406,7 +3410,7 @@
         <v>1.05551732784983</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A123">
         <v>9</v>
       </c>
@@ -3423,7 +3427,7 @@
         <v>1.09151498112135</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A124">
         <v>1</v>
       </c>
@@ -3440,7 +3444,7 @@
         <v>1.1249387366082999</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A125">
         <v>2</v>
       </c>
@@ -3457,7 +3461,7 @@
         <v>1.2441251443275001</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A126">
         <v>3</v>
       </c>
@@ -3474,7 +3478,7 @@
         <v>1.2839966563652001</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A127">
         <v>7</v>
       </c>
@@ -3491,7 +3495,7 @@
         <v>1.36653154442041</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A128">
         <v>1</v>
       </c>
@@ -3508,7 +3512,7 @@
         <v>1.4436974992327101</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A129">
         <v>1</v>
       </c>
@@ -3525,7 +3529,7 @@
         <v>1.46852108295774</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A130">
         <v>1</v>
       </c>
@@ -3542,7 +3546,7 @@
         <v>1.5376020021010399</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A131">
         <v>1</v>
       </c>
@@ -3559,7 +3563,7 @@
         <v>1.58502665202918</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A132">
         <v>161</v>
       </c>
@@ -3576,7 +3580,7 @@
         <v>1.6197887582883901</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A133">
         <v>29</v>
       </c>
@@ -3593,7 +3597,7 @@
         <v>1.6197887582883901</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A134">
         <v>1</v>
       </c>
@@ -3610,7 +3614,7 @@
         <v>1.6382721639824001</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A135">
         <v>7</v>
       </c>
@@ -3627,7 +3631,7 @@
         <v>1.6989700043360101</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A136">
         <v>107</v>
       </c>
@@ -3644,7 +3648,7 @@
         <v>1.8860566476931599</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A137">
         <v>2</v>
       </c>
@@ -3661,7 +3665,7 @@
         <v>1.8860566476931599</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A138">
         <v>11</v>
       </c>
@@ -3678,7 +3682,7 @@
         <v>2.3979400086720299</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A139">
         <v>10</v>
       </c>
@@ -3696,7 +3700,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E140">
+  <sortState ref="A2:E140">
     <sortCondition ref="E2:E140"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3707,81 +3711,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="2">
         <v>25</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>-0.55041549888957597</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>2E-3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>-2.6989700043360099</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>-0.99666846749504701</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2E-3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>-2.6989700043360099</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
         <v>31</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>-0.54642102724421504</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>2E-3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>-2.6989700043360099</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>34</v>
       </c>
@@ -3798,7 +3800,7 @@
         <v>-2.3979400086720299</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3815,7 +3817,7 @@
         <v>-2.3979400086720299</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>4</v>
       </c>
@@ -3832,7 +3834,7 @@
         <v>-1.8860566476931599</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>15</v>
       </c>
@@ -3849,7 +3851,7 @@
         <v>-1.82390874094431</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3866,7 +3868,7 @@
         <v>-1.74472749489669</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3883,7 +3885,7 @@
         <v>-1.4559319556497201</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>3</v>
       </c>
@@ -3900,7 +3902,7 @@
         <v>-1.4202164033831799</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3917,7 +3919,7 @@
         <v>-1.4089353929735</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3934,7 +3936,7 @@
         <v>-1.4089353929735</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3951,7 +3953,7 @@
         <v>-1.3565473235138099</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>1</v>
       </c>
@@ -3968,7 +3970,7 @@
         <v>-1.27572413039921</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3985,7 +3987,7 @@
         <v>-1.21467016498923</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>1</v>
       </c>
@@ -4002,7 +4004,7 @@
         <v>-1.21467016498923</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>2</v>
       </c>
@@ -4019,7 +4021,7 @@
         <v>-1.1870866433571401</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>1</v>
       </c>
@@ -4036,7 +4038,7 @@
         <v>-1.1870866433571401</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -4053,7 +4055,7 @@
         <v>-1.13076828026902</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>3</v>
       </c>
@@ -4070,7 +4072,7 @@
         <v>-1.13076828026902</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>2</v>
       </c>
@@ -4087,7 +4089,7 @@
         <v>-1.1079053973095101</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>5</v>
       </c>
@@ -4104,7 +4106,7 @@
         <v>-1.09691001300805</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -4121,7 +4123,7 @@
         <v>-1.08092190762392</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>8</v>
       </c>
@@ -4138,7 +4140,7 @@
         <v>-1.0506099933550801</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>14</v>
       </c>
@@ -4155,7 +4157,7 @@
         <v>-1.0315170514460601</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -4172,7 +4174,7 @@
         <v>-0.99567862621735703</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -4189,7 +4191,7 @@
         <v>-0.93554201077308097</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>1</v>
       </c>
@@ -4206,7 +4208,7 @@
         <v>-0.920818753952375</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -4223,7 +4225,7 @@
         <v>-0.91721462968354905</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2</v>
       </c>
@@ -4240,7 +4242,7 @@
         <v>-0.88605664769316295</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>1</v>
       </c>
@@ -4257,7 +4259,7 @@
         <v>-0.86012091359876297</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>2</v>
       </c>
@@ -4274,7 +4276,7 @@
         <v>-0.79588001734407499</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>11</v>
       </c>
@@ -4291,7 +4293,7 @@
         <v>-0.75202673363819295</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>1</v>
       </c>
@@ -4308,7 +4310,7 @@
         <v>-0.74714696902010602</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>3</v>
       </c>
@@ -4325,7 +4327,7 @@
         <v>-0.72353819582675505</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>2</v>
       </c>
@@ -4342,7 +4344,7 @@
         <v>-0.67162039656126205</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>1</v>
       </c>
@@ -4359,7 +4361,7 @@
         <v>-0.67162039656126205</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>2</v>
       </c>
@@ -4376,7 +4378,7 @@
         <v>-0.66756154008439395</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>48</v>
       </c>
@@ -4393,7 +4395,7 @@
         <v>-0.66154350639539505</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>4</v>
       </c>
@@ -4410,7 +4412,7 @@
         <v>-0.651695136951839</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>21</v>
       </c>
@@ -4427,7 +4429,7 @@
         <v>-0.64589156085259902</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>2</v>
       </c>
@@ -4444,7 +4446,7 @@
         <v>-0.64206515299954603</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>1</v>
       </c>
@@ -4461,7 +4463,7 @@
         <v>-0.63451201510910005</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>1</v>
       </c>
@@ -4478,7 +4480,7 @@
         <v>-0.56066730616973703</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>2</v>
       </c>
@@ -4495,7 +4497,7 @@
         <v>-0.54060751224076897</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>3</v>
       </c>
@@ -4512,7 +4514,7 @@
         <v>-0.53017798402183702</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>1</v>
       </c>
@@ -4529,7 +4531,7 @@
         <v>-0.52287874528033695</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>2</v>
       </c>
@@ -4546,7 +4548,7 @@
         <v>-0.51144928349955499</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>7</v>
       </c>
@@ -4563,7 +4565,7 @@
         <v>-0.496209316942818</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>2</v>
       </c>
@@ -4580,7 +4582,7 @@
         <v>-0.48678239993206002</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>6</v>
       </c>
@@ -4597,7 +4599,7 @@
         <v>-0.47366072261015502</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>1</v>
       </c>
@@ -4614,7 +4616,7 @@
         <v>-0.43770713554352503</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>1</v>
       </c>
@@ -4631,7 +4633,7 @@
         <v>-0.43533393574791002</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>2</v>
       </c>
@@ -4648,7 +4650,7 @@
         <v>-0.42481215507233799</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>1</v>
       </c>
@@ -4665,7 +4667,7 @@
         <v>-0.41680122603137698</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>2</v>
       </c>
@@ -4682,7 +4684,7 @@
         <v>-0.41453927049149902</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>5</v>
       </c>
@@ -4699,7 +4701,7 @@
         <v>-0.41341269532824498</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>2</v>
       </c>
@@ -4716,7 +4718,7 @@
         <v>-0.40230481407448698</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>1</v>
       </c>
@@ -4733,7 +4735,7 @@
         <v>-0.40120949323688399</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>1</v>
       </c>
@@ -4750,7 +4752,7 @@
         <v>-0.39254497678533101</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>1</v>
       </c>
@@ -4767,7 +4769,7 @@
         <v>-0.37778597703370398</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>2</v>
       </c>
@@ -4784,7 +4786,7 @@
         <v>-0.36151074304536202</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>1</v>
       </c>
@@ -4801,7 +4803,7 @@
         <v>-0.35359627377692998</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>4</v>
       </c>
@@ -4818,7 +4820,7 @@
         <v>-0.33818731446273798</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>5</v>
       </c>
@@ -4835,7 +4837,7 @@
         <v>-0.325138859262188</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>1</v>
       </c>
@@ -4852,7 +4854,7 @@
         <v>-0.31785492362616802</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>1</v>
       </c>
@@ -4869,7 +4871,7 @@
         <v>-0.31247103878536497</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>1</v>
       </c>
@@ -4886,7 +4888,7 @@
         <v>-0.30980391997148599</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>11</v>
       </c>
@@ -4903,7 +4905,7 @@
         <v>0.30980391997148599</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>8</v>
       </c>
@@ -4920,7 +4922,7 @@
         <v>0.31247103878536497</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>1</v>
       </c>
@@ -4937,7 +4939,7 @@
         <v>0.32239304727950602</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>11</v>
       </c>
@@ -4954,7 +4956,7 @@
         <v>0.32330639037513298</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>1</v>
       </c>
@@ -4971,7 +4973,7 @@
         <v>0.33535802444387403</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>14</v>
       </c>
@@ -4988,7 +4990,7 @@
         <v>0.34294414714289601</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>1</v>
       </c>
@@ -5005,7 +5007,7 @@
         <v>0.34294414714289601</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>32</v>
       </c>
@@ -5022,7 +5024,7 @@
         <v>0.36451625318508701</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>1</v>
       </c>
@@ -5039,7 +5041,7 @@
         <v>0.38195190328790701</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>1</v>
       </c>
@@ -5056,7 +5058,7 @@
         <v>0.38615817812393</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>2</v>
       </c>
@@ -5073,7 +5075,7 @@
         <v>0.399027104313251</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>1</v>
       </c>
@@ -5090,7 +5092,7 @@
         <v>0.41116827440579201</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>1</v>
       </c>
@@ -5107,7 +5109,7 @@
         <v>0.427128397799519</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>1</v>
       </c>
@@ -5124,7 +5126,7 @@
         <v>0.42829116819131202</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>8</v>
       </c>
@@ -5141,7 +5143,7 @@
         <v>0.43179827593300502</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>13</v>
       </c>
@@ -5158,7 +5160,7 @@
         <v>0.436518914605589</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>2</v>
       </c>
@@ -5175,7 +5177,7 @@
         <v>0.455931955649724</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>2</v>
       </c>
@@ -5192,7 +5194,7 @@
         <v>0.49894073778224801</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>2</v>
       </c>
@@ -5209,7 +5211,7 @@
         <v>0.53313237964589</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>1</v>
       </c>
@@ -5226,7 +5228,7 @@
         <v>0.53760200210104303</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>4</v>
       </c>
@@ -5243,7 +5245,7 @@
         <v>0.54668165995296203</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>4</v>
       </c>
@@ -5260,7 +5262,7 @@
         <v>0.55284196865778001</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>1</v>
       </c>
@@ -5277,7 +5279,7 @@
         <v>0.57511836336893296</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>4</v>
       </c>
@@ -5294,7 +5296,7 @@
         <v>0.58004425151024197</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>1</v>
       </c>
@@ -5311,7 +5313,7 @@
         <v>0.58838029403676895</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>2</v>
       </c>
@@ -5328,7 +5330,7 @@
         <v>0.59176003468814997</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>2</v>
       </c>
@@ -5345,7 +5347,7 @@
         <v>0.59687947882418202</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>1</v>
       </c>
@@ -5362,7 +5364,7 @@
         <v>0.60906489289662002</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>1</v>
       </c>
@@ -5379,7 +5381,7 @@
         <v>0.62893213772826295</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>1</v>
       </c>
@@ -5396,7 +5398,7 @@
         <v>0.63078414258985704</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>8</v>
       </c>
@@ -5413,7 +5415,7 @@
         <v>0.63451201510910005</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>10</v>
       </c>
@@ -5430,7 +5432,7 @@
         <v>0.63451201510910005</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>11</v>
       </c>
@@ -5447,7 +5449,7 @@
         <v>0.636388020107855</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>2</v>
       </c>
@@ -5464,7 +5466,7 @@
         <v>0.64589156085259902</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>1</v>
       </c>
@@ -5481,7 +5483,7 @@
         <v>0.66354026615146999</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>3</v>
       </c>
@@ -5498,7 +5500,7 @@
         <v>0.66958622665080902</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>4</v>
       </c>
@@ -5515,7 +5517,7 @@
         <v>0.69036983257410101</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>1</v>
       </c>
@@ -5532,7 +5534,7 @@
         <v>0.694648630553376</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>1</v>
       </c>
@@ -5549,7 +5551,7 @@
         <v>0.72353819582675505</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>2</v>
       </c>
@@ -5566,7 +5568,7 @@
         <v>0.73048705578208295</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A110">
         <v>1</v>
       </c>
@@ -5583,7 +5585,7 @@
         <v>0.73992861201492499</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>4</v>
       </c>
@@ -5600,7 +5602,7 @@
         <v>0.74472749489669399</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>1</v>
       </c>
@@ -5617,7 +5619,7 @@
         <v>0.74957999769110595</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A113">
         <v>7</v>
       </c>
@@ -5634,7 +5636,7 @@
         <v>0.75448733218584996</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A114">
         <v>1</v>
       </c>
@@ -5651,7 +5653,7 @@
         <v>0.80410034759076598</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A115">
         <v>2</v>
       </c>
@@ -5668,7 +5670,7 @@
         <v>0.80687540164553795</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A116">
         <v>27</v>
       </c>
@@ -5685,7 +5687,7 @@
         <v>0.81815641205522704</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A117">
         <v>3</v>
       </c>
@@ -5702,7 +5704,7 @@
         <v>0.82390874094431799</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A118">
         <v>2</v>
       </c>
@@ -5719,7 +5721,7 @@
         <v>0.82681373158772598</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>7</v>
       </c>
@@ -5736,7 +5738,7 @@
         <v>0.832682665251823</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A120">
         <v>2</v>
       </c>
@@ -5753,7 +5755,7 @@
         <v>0.84466396253493803</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A121">
         <v>1</v>
       </c>
@@ -5770,7 +5772,7 @@
         <v>0.85078088734461998</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A122">
         <v>2</v>
       </c>
@@ -5787,7 +5789,7 @@
         <v>0.892790030352131</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A123">
         <v>5</v>
       </c>
@@ -5804,7 +5806,7 @@
         <v>0.90657831483776496</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A124">
         <v>1</v>
       </c>
@@ -5821,7 +5823,7 @@
         <v>0.91009488856060194</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A125">
         <v>3</v>
       </c>
@@ -5838,7 +5840,7 @@
         <v>0.920818753952375</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A126">
         <v>5</v>
       </c>
@@ -5855,7 +5857,7 @@
         <v>0.95467702121334197</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A127">
         <v>1</v>
       </c>
@@ -5872,7 +5874,7 @@
         <v>0.96257350205937597</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A128">
         <v>1</v>
       </c>
@@ -5889,7 +5891,7 @@
         <v>0.99567862621735703</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A129">
         <v>1</v>
       </c>
@@ -5906,7 +5908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A130">
         <v>37</v>
       </c>
@@ -5923,7 +5925,7 @@
         <v>1.08618614761628</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A131">
         <v>1</v>
       </c>
@@ -5940,7 +5942,7 @@
         <v>1.1079053973095101</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A132">
         <v>3</v>
       </c>
@@ -5957,7 +5959,7 @@
         <v>1.1191864077192</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A133">
         <v>1</v>
       </c>
@@ -5974,7 +5976,7 @@
         <v>1.1366771398795401</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A134">
         <v>1</v>
       </c>
@@ -5991,7 +5993,7 @@
         <v>1.1366771398795401</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A135">
         <v>1</v>
       </c>
@@ -6008,7 +6010,7 @@
         <v>1.19382002601611</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A136">
         <v>2</v>
       </c>
@@ -6025,7 +6027,7 @@
         <v>1.2218487496163499</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A137">
         <v>1</v>
       </c>
@@ -6042,7 +6044,7 @@
         <v>1.25181197299379</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A138">
         <v>2</v>
       </c>
@@ -6059,7 +6061,7 @@
         <v>1.32790214206428</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A139">
         <v>1</v>
       </c>
@@ -6076,7 +6078,7 @@
         <v>1.3467874862246501</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A140">
         <v>2</v>
       </c>
@@ -6093,7 +6095,7 @@
         <v>1.5376020021010399</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A141">
         <v>8</v>
       </c>
@@ -6110,7 +6112,7 @@
         <v>1.67778070526608</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A142">
         <v>17</v>
       </c>
@@ -6127,7 +6129,7 @@
         <v>1.92081875395237</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A143">
         <v>1</v>
       </c>
@@ -6144,7 +6146,7 @@
         <v>2.5228787452803298</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A144">
         <v>112</v>
       </c>
@@ -6161,7 +6163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A145">
         <v>179</v>
       </c>
@@ -6178,7 +6180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A146">
         <v>2</v>
       </c>
@@ -6196,7 +6198,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E147">
+  <sortState ref="A2:E147">
     <sortCondition ref="E2:E147"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>